<commit_message>
2023 test 2 part 1 -2
</commit_message>
<xml_diff>
--- a/Toeic Test Result.xlsx
+++ b/Toeic Test Result.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\Private\Github\Learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAE01A3-553A-4073-A957-918252F62278}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F55A347-16BF-41CF-89A7-FCF7350A8F92}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{12AD4287-8134-4218-AA5C-6842D8F962AE}"/>
   </bookViews>
   <sheets>
     <sheet name="2023_test 1" sheetId="1" r:id="rId1"/>
-    <sheet name="part 7" sheetId="2" r:id="rId2"/>
+    <sheet name="2023_test 2" sheetId="3" r:id="rId2"/>
+    <sheet name="part 7" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -285,7 +286,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="40">
   <si>
     <t>C</t>
   </si>
@@ -321,13 +322,97 @@
   </si>
   <si>
     <t xml:space="preserve">mục đích chính của bài viết </t>
+  </si>
+  <si>
+    <t>Avoid</t>
+  </si>
+  <si>
+    <t>Allow</t>
+  </si>
+  <si>
+    <t>Consider</t>
+  </si>
+  <si>
+    <t>Delay</t>
+  </si>
+  <si>
+    <t>Dislike</t>
+  </si>
+  <si>
+    <t>Appreciate</t>
+  </si>
+  <si>
+    <t>Enjoy</t>
+  </si>
+  <si>
+    <t>Anticipate</t>
+  </si>
+  <si>
+    <t>Begin</t>
+  </si>
+  <si>
+    <t>Discuss</t>
+  </si>
+  <si>
+    <t>Finish</t>
+  </si>
+  <si>
+    <t>Admit</t>
+  </si>
+  <si>
+    <t>Advise</t>
+  </si>
+  <si>
+    <t>Agree</t>
+  </si>
+  <si>
+    <t>ASK</t>
+  </si>
+  <si>
+    <t>Keep</t>
+  </si>
+  <si>
+    <t>Afford</t>
+  </si>
+  <si>
+    <t>Appear</t>
+  </si>
+  <si>
+    <t>Arrange</t>
+  </si>
+  <si>
+    <t>Defend</t>
+  </si>
+  <si>
+    <t>Hope</t>
+  </si>
+  <si>
+    <t>Learn</t>
+  </si>
+  <si>
+    <t>Attempt</t>
+  </si>
+  <si>
+    <t>Bear</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -356,13 +441,66 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="4"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF7030A0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF7030A0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -377,9 +515,34 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -789,8 +952,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{655F0DDF-1B32-46C2-9216-2FC55073B863}">
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="F33" sqref="F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1458,11 +1621,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{845C02CE-50F4-4AF0-B9FF-45AB471D7261}">
+  <dimension ref="A1:E31"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="8.7265625" style="10"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="9">
+        <v>45455</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>38</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>37</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>37</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" s="11" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A31" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B31" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A8A6E05-AFDB-4E96-9660-A36DCBDB4DF8}">
-  <dimension ref="A2:B2"/>
+  <dimension ref="A2:F50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1475,7 +1828,169 @@
         <v>11</v>
       </c>
     </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B27" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B28" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B29" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D29" s="7"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B30" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C30" s="4"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B31" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" s="4"/>
+      <c r="E31" s="7"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E32" s="7"/>
+      <c r="F32" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B33" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C33" s="4"/>
+      <c r="E33" s="8"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B34" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C34" s="4"/>
+      <c r="D34" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E34" s="7"/>
+      <c r="F34" s="5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B35" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C35" s="7"/>
+      <c r="E35" s="7"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B36" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="7"/>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C37" s="7"/>
+      <c r="D37" s="7"/>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B38" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7"/>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B39" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B40" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B41" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B42" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B45" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B46" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B47" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.35">
+      <c r="B48" s="2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B49" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B50" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B27:B50">
+    <sortCondition ref="B27:B50"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>